<commit_message>
Falsche Regressionen für Lilienthal Polare korrigiert
</commit_message>
<xml_diff>
--- a/Unterlagen/Do128 Berechnungen & Plots.xlsx
+++ b/Unterlagen/Do128 Berechnungen & Plots.xlsx
@@ -295,7 +295,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="25400" cap="rnd">
               <a:noFill/>
               <a:round/>
             </a:ln>
@@ -329,15 +329,15 @@
             </c:spPr>
             <c:trendlineType val="poly"/>
             <c:order val="2"/>
-            <c:forward val="6.0000000000000012E-2"/>
-            <c:backward val="1.0000000000000002E-2"/>
+            <c:forward val="1"/>
+            <c:backward val="0.4"/>
             <c:dispRSqr val="0"/>
             <c:dispEq val="1"/>
             <c:trendlineLbl>
               <c:layout>
                 <c:manualLayout>
-                  <c:x val="-7.4715350846630895E-3"/>
-                  <c:y val="0.45314813524415642"/>
+                  <c:x val="-0.14289512925928508"/>
+                  <c:y val="-7.2894339534991748E-2"/>
                 </c:manualLayout>
               </c:layout>
               <c:tx>
@@ -363,12 +363,16 @@
                       <a:t>C</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1100" baseline="0"/>
-                      <a:t>w</a:t>
+                      <a:rPr lang="en-US" sz="1050" baseline="0"/>
+                      <a:t>W</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                      <a:t> = -164 Ca </a:t>
+                      <a:t> = 0,0228 C</a:t>
+                    </a:r>
+                    <a:r>
+                      <a:rPr lang="en-US" sz="1050" baseline="0"/>
+                      <a:t>A</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1400" baseline="30000"/>
@@ -376,23 +380,15 @@
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                      <a:t> + 48,7 </a:t>
+                      <a:t> + 0,0041 C</a:t>
                     </a:r>
                     <a:r>
-                      <a:rPr lang="en-US" sz="1400" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:effectLst/>
-                      </a:rPr>
-                      <a:t>C</a:t>
-                    </a:r>
-                    <a:r>
-                      <a:rPr lang="en-US" sz="1100" b="0" i="0" u="none" strike="noStrike" baseline="0">
-                        <a:effectLst/>
-                      </a:rPr>
-                      <a:t>a</a:t>
+                      <a:rPr lang="en-US" sz="1050" baseline="0"/>
+                      <a:t>A</a:t>
                     </a:r>
                     <a:r>
                       <a:rPr lang="en-US" sz="1400" baseline="0"/>
-                      <a:t> - 1,9</a:t>
+                      <a:t> + 0,056</a:t>
                     </a:r>
                     <a:endParaRPr lang="en-US" sz="1400"/>
                   </a:p>
@@ -430,6 +426,27 @@
           </c:trendline>
           <c:xVal>
             <c:numRef>
+              <c:f>Kenngrößen!$D$27:$D$30</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="4"/>
+                <c:pt idx="0">
+                  <c:v>1.4368888640934547</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.91648470139471716</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.63400373966358547</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.46308050886070595</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
               <c:f>Kenngrößen!$C$27:$C$30</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
@@ -445,27 +462,6 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>6.3836498081065979E-2</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:xVal>
-          <c:yVal>
-            <c:numRef>
-              <c:f>Kenngrößen!$D$27:$D$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
-                <c:pt idx="0">
-                  <c:v>1.4368888640934547</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>0.91648470139471716</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>0.63400373966358547</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>0.46308050886070595</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -492,6 +488,7 @@
         <c:axId val="1463035759"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="2.5"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -530,7 +527,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1400"/>
-                  <a:t>Widerstandsbeiwert Cw</a:t>
+                  <a:t>Auftriebsbeiwert CA</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -648,7 +645,7 @@
                 </a:pPr>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1400"/>
-                  <a:t>Auftriebsbeiwert</a:t>
+                  <a:t>Widerstandsbeiwert</a:t>
                 </a:r>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1400" baseline="0"/>
@@ -660,7 +657,7 @@
                 </a:r>
                 <a:r>
                   <a:rPr lang="de-DE" sz="1050"/>
-                  <a:t>A</a:t>
+                  <a:t>W</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -2941,8 +2938,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:P60"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27:D30"/>
+    <sheetView tabSelected="1" topLeftCell="F13" zoomScale="190" zoomScaleNormal="190" workbookViewId="0">
+      <selection activeCell="O17" sqref="O17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>